<commit_message>
Second Entry in demo file
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SECI\SECI\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C688AE54-AD38-4630-9204-79634637B406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697E65F5-2CF3-4950-81EC-DD306485F697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4896" yWindow="4920" windowWidth="23040" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Arihant Jammar</t>
+  </si>
+  <si>
+    <t>Ronit Jammar</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,6 +382,14 @@
         <v>9137456073</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>9257202428</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>